<commit_message>
Add SQL script to calculate monthly percentage increase in COVID-19 cases
</commit_message>
<xml_diff>
--- a/Covid_Percentage_Increase/Problem_Statement.xlsx
+++ b/Covid_Percentage_Increase/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q16/Video_Q16_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Covid_Percentage_Increase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7820C4DA-C560-E84F-83CC-8E1D475675EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF752AD-0C09-4F0D-8211-133FBAF44A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{1B75FF4D-71F2-414D-A495-BCE200FA4A08}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{1B75FF4D-71F2-414D-A495-BCE200FA4A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -59,9 +57,6 @@
     <t>OUTPUT</t>
   </si>
   <si>
-    <t>Video #16 - Covid Percentage Increase</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -84,6 +79,9 @@
 Calculate the percentage increase in covid cases each month versus cumulative cases as of the prior month.
 Return the month number, and the percentage increase rounded to one decimal. Order the result by the month.</t>
     </r>
+  </si>
+  <si>
+    <t># - Covid Percentage Increase</t>
   </si>
 </sst>
 </file>
@@ -323,61 +321,61 @@
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,514 +713,514 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B77357-9687-E443-9898-79AC8D857BAD}">
   <dimension ref="B1:G48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="13.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="20.796875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="13.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" style="1"/>
+    <col min="6" max="6" width="13.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:7" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="2:7" s="16" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="2:7" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="2:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="2:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="2:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="7" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="17"/>
+      <c r="F8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
+        <v>20124</v>
+      </c>
+      <c r="C10" s="7">
+        <v>43840</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="9">
+        <v>40133</v>
+      </c>
+      <c r="C11" s="10">
+        <v>43845</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="F11" s="9">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="9">
+        <v>65005</v>
+      </c>
+      <c r="C12" s="10">
+        <v>43850</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="F12" s="9">
+        <v>3</v>
+      </c>
+      <c r="G12" s="11">
+        <v>148.9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
+        <v>30005</v>
+      </c>
+      <c r="C13" s="10">
+        <v>43869</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="F13" s="9">
+        <v>4</v>
+      </c>
+      <c r="G13" s="11">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="9">
+        <v>35015</v>
+      </c>
+      <c r="C14" s="10">
+        <v>43880</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="F14" s="9">
+        <v>5</v>
+      </c>
+      <c r="G14" s="11">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="9">
+        <v>15015</v>
+      </c>
+      <c r="C15" s="10">
+        <v>43893</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="F15" s="9">
+        <v>6</v>
+      </c>
+      <c r="G15" s="11">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="9">
+        <v>35035</v>
+      </c>
+      <c r="C16" s="10">
+        <v>43900</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="F16" s="9">
+        <v>7</v>
+      </c>
+      <c r="G16" s="11">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="9">
+        <v>49099</v>
+      </c>
+      <c r="C17" s="10">
+        <v>43904</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="F17" s="9">
         <v>8</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="2:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="2:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-    </row>
-    <row r="5" spans="2:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="7" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="21"/>
-      <c r="F8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="F9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="8">
-        <v>20124</v>
-      </c>
-      <c r="C10" s="9">
-        <v>43840</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="11">
-        <v>40133</v>
-      </c>
-      <c r="C11" s="12">
-        <v>43845</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="F11" s="11">
-        <v>2</v>
-      </c>
-      <c r="G11" s="13">
-        <v>51.9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="11">
-        <v>65005</v>
-      </c>
-      <c r="C12" s="12">
-        <v>43850</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="F12" s="11">
-        <v>3</v>
-      </c>
-      <c r="G12" s="13">
-        <v>148.9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="11">
-        <v>30005</v>
-      </c>
-      <c r="C13" s="12">
-        <v>43869</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="F13" s="11">
-        <v>4</v>
-      </c>
-      <c r="G13" s="13">
-        <v>61.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="11">
-        <v>35015</v>
-      </c>
-      <c r="C14" s="12">
-        <v>43880</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="F14" s="11">
-        <v>5</v>
-      </c>
-      <c r="G14" s="13">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="11">
-        <v>15015</v>
-      </c>
-      <c r="C15" s="12">
-        <v>43893</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="F15" s="11">
-        <v>6</v>
-      </c>
-      <c r="G15" s="13">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="11">
-        <v>35035</v>
-      </c>
-      <c r="C16" s="12">
-        <v>43900</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="F16" s="11">
-        <v>7</v>
-      </c>
-      <c r="G16" s="13">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="11">
-        <v>49099</v>
-      </c>
-      <c r="C17" s="12">
-        <v>43904</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="F17" s="11">
-        <v>8</v>
-      </c>
-      <c r="G17" s="13">
+      <c r="G17" s="11">
         <v>3.9</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="11">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="9">
         <v>84045</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="10">
         <v>43910</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="F18" s="11">
+      <c r="D18" s="17"/>
+      <c r="F18" s="9">
         <v>9</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="11">
         <v>7.9</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="11">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="9">
         <v>100106</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="10">
         <v>43921</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="F19" s="11">
+      <c r="D19" s="17"/>
+      <c r="F19" s="9">
         <v>10</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="11">
         <v>1.7</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="11">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="9">
         <v>17015</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="10">
         <v>43925</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="F20" s="11">
+      <c r="D20" s="17"/>
+      <c r="F20" s="9">
         <v>11</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="11">
         <v>6.4</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11">
+    <row r="21" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="9">
         <v>36035</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="10">
         <v>43932</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="F21" s="14">
+      <c r="D21" s="17"/>
+      <c r="F21" s="12">
         <v>12</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="13">
         <v>7.4</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="11">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="9">
         <v>50099</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="10">
         <v>43934</v>
       </c>
-      <c r="D22" s="21"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="11">
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="9">
         <v>87045</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="10">
         <v>43943</v>
       </c>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="11">
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="9">
         <v>101101</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="10">
         <v>43951</v>
       </c>
-      <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="11">
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="9">
         <v>40015</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="10">
         <v>43952</v>
       </c>
-      <c r="D25" s="21"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="11">
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="9">
         <v>54035</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="10">
         <v>43960</v>
       </c>
-      <c r="D26" s="21"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="11">
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="9">
         <v>71099</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="10">
         <v>43965</v>
       </c>
-      <c r="D27" s="21"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="11">
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="9">
         <v>82045</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="10">
         <v>43972</v>
       </c>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="11">
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="9">
         <v>90103</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="10">
         <v>43976</v>
       </c>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="11">
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="9">
         <v>99103</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="10">
         <v>43982</v>
       </c>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="11">
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="9">
         <v>11015</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="10">
         <v>43985</v>
       </c>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="11">
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="9">
         <v>28035</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="10">
         <v>43992</v>
       </c>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="11">
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="9">
         <v>38099</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="10">
         <v>43996</v>
       </c>
-      <c r="D33" s="21"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="11">
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="9">
         <v>45045</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="10">
         <v>44002</v>
       </c>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="11">
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="9">
         <v>36033</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="10">
         <v>44021</v>
       </c>
-      <c r="D35" s="21"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="11">
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="9">
         <v>40011</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="10">
         <v>44035</v>
       </c>
-      <c r="D36" s="21"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="11">
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="9">
         <v>25001</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="10">
         <v>44055</v>
       </c>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="11">
+      <c r="D37" s="17"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="9">
         <v>29990</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="10">
         <v>44069</v>
       </c>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="11">
+      <c r="D38" s="17"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="9">
         <v>20112</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="10">
         <v>44078</v>
       </c>
-      <c r="D39" s="21"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="11">
+      <c r="D39" s="17"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="9">
         <v>43991</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="10">
         <v>44092</v>
       </c>
-      <c r="D40" s="21"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="11">
+      <c r="D40" s="17"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="9">
         <v>51002</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="10">
         <v>44103</v>
       </c>
-      <c r="D41" s="21"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="11">
+      <c r="D41" s="17"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="9">
         <v>26587</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="10">
         <v>44129</v>
       </c>
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="11">
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="9">
         <v>11000</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="10">
         <v>44142</v>
       </c>
-      <c r="D43" s="21"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="11">
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="9">
         <v>35002</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="10">
         <v>44151</v>
       </c>
-      <c r="D44" s="21"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="11">
+      <c r="D44" s="17"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="9">
         <v>56010</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="10">
         <v>44163</v>
       </c>
-      <c r="D45" s="21"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="11">
+      <c r="D45" s="17"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="9">
         <v>15099</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="10">
         <v>44167</v>
       </c>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="11">
+      <c r="D46" s="17"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="9">
         <v>38042</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="10">
         <v>44176</v>
       </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14">
+      <c r="D47" s="17"/>
+    </row>
+    <row r="48" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="12">
         <v>73030</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="14">
         <v>44191</v>
       </c>
-      <c r="D48" s="21"/>
+      <c r="D48" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1232,5 +1230,6 @@
     <mergeCell ref="B2:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>